<commit_message>
Backup QR Scanner data - 2025-12-17T06:42:33.532Z - Cache Bust: 1765953753532
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Histology_scanner1765953517799_198f95adaaec95b0d36c4caac83d14ce8169b0e9e2b4e7780eb0fc4436173541.xlsx
+++ b/log_history/Y2_B2526_Histology_scanner1765953517799_198f95adaaec95b0d36c4caac83d14ce8169b0e9e2b4e7780eb0fc4436173541.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Session" sheetId="1" r:id="rId1"/>
+    <sheet name="Histology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -602,9 +602,349 @@
         <v>norhan.mohamed@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>241141</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C11" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D11" t="str">
+        <v>08:40:34</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F11" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>241142</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C12" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D12" t="str">
+        <v>08:40:39</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F12" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>241143</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C13" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D13" t="str">
+        <v>08:40:42</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F13" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>241198</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C14" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D14" t="str">
+        <v>08:41:23</v>
+      </c>
+      <c r="E14" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F14" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>241118</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C15" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D15" t="str">
+        <v>08:41:32</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F15" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>241175</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C16" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D16" t="str">
+        <v>08:41:35</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F16" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>241177</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C17" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D17" t="str">
+        <v>08:41:39</v>
+      </c>
+      <c r="E17" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F17" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>241178</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C18" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D18" t="str">
+        <v>08:41:41</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F18" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>241153</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C19" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D19" t="str">
+        <v>08:41:48</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F19" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>241206</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C20" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D20" t="str">
+        <v>08:41:53</v>
+      </c>
+      <c r="E20" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F20" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>241197</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C21" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D21" t="str">
+        <v>08:41:57</v>
+      </c>
+      <c r="E21" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F21" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>241103</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C22" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D22" t="str">
+        <v>08:42:01</v>
+      </c>
+      <c r="E22" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F22" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>241104</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C23" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D23" t="str">
+        <v>08:42:04</v>
+      </c>
+      <c r="E23" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F23" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>241132</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C24" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D24" t="str">
+        <v>08:42:08</v>
+      </c>
+      <c r="E24" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F24" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>241144</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C25" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D25" t="str">
+        <v>08:42:12</v>
+      </c>
+      <c r="E25" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F25" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>241228</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C26" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D26" t="str">
+        <v>08:42:15</v>
+      </c>
+      <c r="E26" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F26" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>241045</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C27" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D27" t="str">
+        <v>08:42:27</v>
+      </c>
+      <c r="E27" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F27" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Backup QR Scanner data - 2025-12-17T07:22:10.517Z - Cache Bust: 1765956130517
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Histology_scanner1765953517799_198f95adaaec95b0d36c4caac83d14ce8169b0e9e2b4e7780eb0fc4436173541.xlsx
+++ b/log_history/Y2_B2526_Histology_scanner1765953517799_198f95adaaec95b0d36c4caac83d14ce8169b0e9e2b4e7780eb0fc4436173541.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -942,9 +942,729 @@
         <v>norhan.mohamed@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>241220</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C28" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D28" t="str">
+        <v>08:42:30</v>
+      </c>
+      <c r="E28" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F28" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>241156</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C29" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D29" t="str">
+        <v>08:42:33</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F29" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>241160</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C30" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D30" t="str">
+        <v>08:42:37</v>
+      </c>
+      <c r="E30" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F30" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>241212</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C31" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D31" t="str">
+        <v>08:42:40</v>
+      </c>
+      <c r="E31" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F31" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>241196</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C32" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D32" t="str">
+        <v>08:42:43</v>
+      </c>
+      <c r="E32" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F32" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>241221</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C33" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D33" t="str">
+        <v>08:42:46</v>
+      </c>
+      <c r="E33" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F33" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>241131</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C34" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D34" t="str">
+        <v>08:42:51</v>
+      </c>
+      <c r="E34" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F34" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>241158</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C35" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D35" t="str">
+        <v>08:42:53</v>
+      </c>
+      <c r="E35" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F35" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>241113</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C36" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D36" t="str">
+        <v>08:43:01</v>
+      </c>
+      <c r="E36" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F36" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>241202</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C37" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D37" t="str">
+        <v>08:43:06</v>
+      </c>
+      <c r="E37" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F37" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>241190</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C38" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D38" t="str">
+        <v>08:43:11</v>
+      </c>
+      <c r="E38" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F38" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>241188</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C39" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D39" t="str">
+        <v>08:43:19</v>
+      </c>
+      <c r="E39" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F39" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>241209</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C40" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D40" t="str">
+        <v>08:43:25</v>
+      </c>
+      <c r="E40" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F40" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>241193</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C41" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D41" t="str">
+        <v>08:43:29</v>
+      </c>
+      <c r="E41" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F41" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>241195</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C42" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D42" t="str">
+        <v>08:43:32</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F42" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>241237</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C43" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D43" t="str">
+        <v>08:43:36</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F43" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>241199</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C44" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D44" t="str">
+        <v>08:43:39</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F44" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>241189</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C45" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D45" t="str">
+        <v>08:43:43</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F45" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>241205</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C46" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D46" t="str">
+        <v>08:43:47</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F46" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>241176</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C47" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D47" t="str">
+        <v>08:43:56</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F47" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>241167</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C48" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D48" t="str">
+        <v>08:43:58</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F48" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>241155</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C49" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D49" t="str">
+        <v>08:44:02</v>
+      </c>
+      <c r="E49" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F49" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>241126</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C50" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D50" t="str">
+        <v>08:44:06</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F50" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>241147</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C51" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D51" t="str">
+        <v>08:44:10</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F51" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>241187</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C52" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D52" t="str">
+        <v>08:44:15</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F52" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>241171</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C53" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D53" t="str">
+        <v>08:44:17</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F53" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>241121</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C54" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D54" t="str">
+        <v>08:44:22</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F54" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>241225</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C55" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D55" t="str">
+        <v>08:44:39</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F55" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>241186</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C56" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D56" t="str">
+        <v>08:44:55</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F56" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>241208</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C57" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D57" t="str">
+        <v>08:45:01</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F57" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>241174</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C58" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D58" t="str">
+        <v>08:45:05</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F58" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>241218</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C59" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D59" t="str">
+        <v>08:46:42</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F59" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>241102</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C60" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D60" t="str">
+        <v>08:46:46</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F60" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>241168</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C61" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D61" t="str">
+        <v>08:46:49</v>
+      </c>
+      <c r="E61" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F61" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>241166</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C62" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D62" t="str">
+        <v>08:46:53</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F62" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>241161</v>
+      </c>
+      <c r="B63" t="str">
+        <v>Histology</v>
+      </c>
+      <c r="C63" t="str">
+        <v>17/12/2025</v>
+      </c>
+      <c r="D63" t="str">
+        <v>08:47:03</v>
+      </c>
+      <c r="E63" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F63" t="str">
+        <v>norhan.mohamed@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F63"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>